<commit_message>
Code Review for Voucher
</commit_message>
<xml_diff>
--- a/tests/artifact/script/Mobile-Voucher.xlsx
+++ b/tests/artifact/script/Mobile-Voucher.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9287" tabRatio="550" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="550" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="825">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="826">
   <si>
     <t>target</t>
   </si>
@@ -2538,6 +2538,9 @@
   </si>
   <si>
     <t>Voucher Created Successfully!</t>
+  </si>
+  <si>
+    <t>Please add all the Voucher related test coverage.</t>
   </si>
 </sst>
 </file>
@@ -2545,13 +2548,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="dd\-mm\-yyyy;@"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="180" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="32">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2605,6 +2608,13 @@
       <sz val="9"/>
       <color rgb="FF1F1F1F"/>
       <name val="Courier New"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Tahoma"/>
       <charset val="134"/>
     </font>
     <font>
@@ -3129,26 +3139,23 @@
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3157,119 +3164,122 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3373,7 +3383,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -3395,6 +3405,10 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3431,7 +3445,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -3443,20 +3457,20 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -3480,15 +3494,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -3857,7 +3871,7 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="18" width="8.33333333333333" customWidth="1" collapsed="1"/>
   </cols>
@@ -6528,13 +6542,13 @@
   <sheetPr/>
   <dimension ref="A1:P225"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="44.5333333333333" style="6" customWidth="1"/>
     <col min="2" max="2" width="42.75" style="7" customWidth="1"/>
@@ -6553,7 +6567,7 @@
     <col min="16" max="16384" width="10.8333333333333" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.15" spans="1:15">
+    <row r="1" ht="15.25" spans="1:15">
       <c r="A1" s="15" t="s">
         <v>725</v>
       </c>
@@ -6575,16 +6589,16 @@
       <c r="I1" s="17" t="s">
         <v>730</v>
       </c>
-      <c r="J1" s="40"/>
-      <c r="K1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="42"/>
       <c r="L1" s="17" t="s">
         <v>731</v>
       </c>
       <c r="M1" s="17"/>
       <c r="N1" s="17"/>
-      <c r="O1" s="42"/>
-    </row>
-    <row r="2" s="1" customFormat="1" ht="15.15" spans="1:15">
+      <c r="O1" s="43"/>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="18" t="s">
         <v>732</v>
       </c>
@@ -6596,12 +6610,12 @@
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
       <c r="I2" s="21"/>
-      <c r="J2" s="43"/>
+      <c r="J2" s="44"/>
       <c r="K2" s="25"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
     </row>
     <row r="3" s="1" customFormat="1" ht="10" customHeight="1" spans="1:15">
       <c r="A3" s="22"/>
@@ -6613,7 +6627,7 @@
       <c r="G3" s="26"/>
       <c r="H3" s="26"/>
       <c r="I3" s="26"/>
-      <c r="J3" s="46"/>
+      <c r="J3" s="47"/>
       <c r="K3" s="25"/>
       <c r="L3" s="26"/>
       <c r="M3" s="24"/>
@@ -6648,10 +6662,10 @@
       <c r="I4" s="27" t="s">
         <v>740</v>
       </c>
-      <c r="J4" s="47" t="s">
+      <c r="J4" s="48" t="s">
         <v>741</v>
       </c>
-      <c r="K4" s="48"/>
+      <c r="K4" s="49"/>
       <c r="L4" s="27" t="s">
         <v>742</v>
       </c>
@@ -6665,7 +6679,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="1" ht="31.2" spans="1:15">
+    <row r="5" s="1" customFormat="1" ht="31" spans="1:15">
       <c r="A5" s="22" t="s">
         <v>746</v>
       </c>
@@ -6681,7 +6695,7 @@
       <c r="E5" s="31" t="s">
         <v>748</v>
       </c>
-      <c r="F5" s="57" t="s">
+      <c r="F5" s="58" t="s">
         <v>749</v>
       </c>
       <c r="G5" s="31"/>
@@ -6694,9 +6708,9 @@
       <c r="N5" s="26"/>
       <c r="O5" s="25"/>
     </row>
-    <row r="6" s="3" customFormat="1" ht="15.6" spans="1:15">
+    <row r="6" s="3" customFormat="1" ht="15.5" spans="1:15">
       <c r="A6" s="22"/>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="59" t="s">
         <v>750</v>
       </c>
       <c r="C6" s="35" t="s">
@@ -6708,7 +6722,7 @@
       <c r="E6" s="31" t="s">
         <v>751</v>
       </c>
-      <c r="F6" s="59" t="s">
+      <c r="F6" s="60" t="s">
         <v>752</v>
       </c>
       <c r="G6" s="31"/>
@@ -6723,7 +6737,7 @@
     </row>
     <row r="7" s="4" customFormat="1" ht="42" customHeight="1" spans="1:15">
       <c r="A7" s="22"/>
-      <c r="B7" s="60"/>
+      <c r="B7" s="61"/>
       <c r="C7" s="28"/>
       <c r="D7" s="29"/>
       <c r="E7" s="29"/>
@@ -6732,11 +6746,11 @@
       <c r="H7" s="29"/>
       <c r="I7" s="29"/>
       <c r="J7" s="37"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="49"/>
-      <c r="O7" s="41"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="42"/>
     </row>
     <row r="8" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A8" s="36"/>
@@ -6749,11 +6763,11 @@
       <c r="H8" s="29"/>
       <c r="I8" s="29"/>
       <c r="J8" s="37"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="49"/>
-      <c r="O8" s="41"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="42"/>
     </row>
     <row r="9" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A9" s="36"/>
@@ -6766,11 +6780,11 @@
       <c r="H9" s="29"/>
       <c r="I9" s="29"/>
       <c r="J9" s="37"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="50"/>
-      <c r="N9" s="49"/>
-      <c r="O9" s="41"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="50"/>
+      <c r="O9" s="42"/>
     </row>
     <row r="10" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A10" s="36"/>
@@ -6783,11 +6797,11 @@
       <c r="H10" s="29"/>
       <c r="I10" s="29"/>
       <c r="J10" s="37"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="49"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="49"/>
-      <c r="O10" s="41"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="50"/>
+      <c r="O10" s="42"/>
     </row>
     <row r="11" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A11" s="36"/>
@@ -6800,11 +6814,11 @@
       <c r="H11" s="29"/>
       <c r="I11" s="29"/>
       <c r="J11" s="37"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="49"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="49"/>
-      <c r="O11" s="41"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="42"/>
     </row>
     <row r="12" s="4" customFormat="1" ht="29" customHeight="1" spans="1:15">
       <c r="A12" s="36"/>
@@ -6817,11 +6831,11 @@
       <c r="H12" s="29"/>
       <c r="I12" s="29"/>
       <c r="J12" s="37"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="49"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="49"/>
-      <c r="O12" s="41"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="42"/>
     </row>
     <row r="13" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A13" s="36"/>
@@ -6834,11 +6848,11 @@
       <c r="H13" s="29"/>
       <c r="I13" s="29"/>
       <c r="J13" s="37"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="49"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="49"/>
-      <c r="O13" s="41"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="42"/>
     </row>
     <row r="14" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A14" s="36"/>
@@ -6851,11 +6865,11 @@
       <c r="H14" s="29"/>
       <c r="I14" s="29"/>
       <c r="J14" s="37"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="49"/>
-      <c r="O14" s="41"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="50"/>
+      <c r="O14" s="42"/>
     </row>
     <row r="15" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A15" s="36"/>
@@ -6868,11 +6882,11 @@
       <c r="H15" s="29"/>
       <c r="I15" s="29"/>
       <c r="J15" s="37"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="49"/>
-      <c r="M15" s="50"/>
-      <c r="N15" s="49"/>
-      <c r="O15" s="41"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="50"/>
+      <c r="O15" s="42"/>
     </row>
     <row r="16" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A16" s="36"/>
@@ -6885,11 +6899,11 @@
       <c r="H16" s="29"/>
       <c r="I16" s="29"/>
       <c r="J16" s="37"/>
-      <c r="K16" s="41"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="50"/>
-      <c r="N16" s="49"/>
-      <c r="O16" s="41"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="50"/>
+      <c r="M16" s="51"/>
+      <c r="N16" s="50"/>
+      <c r="O16" s="42"/>
     </row>
     <row r="17" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A17" s="36"/>
@@ -6902,11 +6916,11 @@
       <c r="H17" s="29"/>
       <c r="I17" s="29"/>
       <c r="J17" s="37"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="50"/>
-      <c r="N17" s="49"/>
-      <c r="O17" s="41"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="50"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="50"/>
+      <c r="O17" s="42"/>
     </row>
     <row r="18" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A18" s="36"/>
@@ -6919,11 +6933,11 @@
       <c r="H18" s="29"/>
       <c r="I18" s="29"/>
       <c r="J18" s="37"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="49"/>
-      <c r="M18" s="50"/>
-      <c r="N18" s="49"/>
-      <c r="O18" s="41"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="50"/>
+      <c r="M18" s="51"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="42"/>
     </row>
     <row r="19" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A19" s="36"/>
@@ -6936,11 +6950,11 @@
       <c r="H19" s="29"/>
       <c r="I19" s="29"/>
       <c r="J19" s="37"/>
-      <c r="K19" s="41"/>
-      <c r="L19" s="49"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="49"/>
-      <c r="O19" s="41"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="50"/>
+      <c r="O19" s="42"/>
     </row>
     <row r="20" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A20" s="36"/>
@@ -6953,11 +6967,11 @@
       <c r="H20" s="29"/>
       <c r="I20" s="29"/>
       <c r="J20" s="37"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="49"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="49"/>
-      <c r="O20" s="41"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="50"/>
+      <c r="O20" s="42"/>
     </row>
     <row r="21" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A21" s="36"/>
@@ -6970,11 +6984,11 @@
       <c r="H21" s="29"/>
       <c r="I21" s="29"/>
       <c r="J21" s="37"/>
-      <c r="K21" s="41"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="50"/>
-      <c r="N21" s="49"/>
-      <c r="O21" s="41"/>
+      <c r="K21" s="42"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="50"/>
+      <c r="O21" s="42"/>
     </row>
     <row r="22" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A22" s="36"/>
@@ -6987,15 +7001,15 @@
       <c r="H22" s="29"/>
       <c r="I22" s="29"/>
       <c r="J22" s="37"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="50"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="41"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="51"/>
+      <c r="N22" s="50"/>
+      <c r="O22" s="42"/>
     </row>
     <row r="23" s="4" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A23" s="36"/>
-      <c r="B23" s="39"/>
+      <c r="B23" s="40"/>
       <c r="C23" s="35"/>
       <c r="D23" s="31"/>
       <c r="E23" s="31"/>
@@ -7004,11 +7018,11 @@
       <c r="H23" s="29"/>
       <c r="I23" s="29"/>
       <c r="J23" s="37"/>
-      <c r="K23" s="41"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="49"/>
-      <c r="O23" s="41"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="51"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="42"/>
     </row>
     <row r="24" s="1" customFormat="1" ht="24" customHeight="1" spans="2:15">
       <c r="B24" s="23"/>
@@ -7063,7 +7077,7 @@
       <c r="B27" s="23"/>
       <c r="C27" s="35"/>
       <c r="D27" s="31"/>
-      <c r="E27" s="61"/>
+      <c r="E27" s="62"/>
       <c r="F27" s="34"/>
       <c r="G27" s="31"/>
       <c r="H27" s="31"/>
@@ -7080,7 +7094,7 @@
       <c r="B28" s="23"/>
       <c r="C28" s="35"/>
       <c r="D28" s="31"/>
-      <c r="E28" s="61"/>
+      <c r="E28" s="62"/>
       <c r="F28" s="30"/>
       <c r="G28" s="31"/>
       <c r="H28" s="31"/>
@@ -7097,7 +7111,7 @@
       <c r="B29" s="23"/>
       <c r="C29" s="35"/>
       <c r="D29" s="31"/>
-      <c r="E29" s="61"/>
+      <c r="E29" s="62"/>
       <c r="F29" s="34"/>
       <c r="G29" s="31"/>
       <c r="H29" s="31"/>
@@ -7114,7 +7128,7 @@
       <c r="B30" s="23"/>
       <c r="C30" s="28"/>
       <c r="D30" s="29"/>
-      <c r="E30" s="61"/>
+      <c r="E30" s="62"/>
       <c r="F30" s="34"/>
       <c r="G30" s="31"/>
       <c r="H30" s="31"/>
@@ -7129,12 +7143,12 @@
     <row r="31" ht="19" customHeight="1" spans="3:6">
       <c r="C31" s="28"/>
       <c r="D31" s="29"/>
-      <c r="F31" s="62"/>
+      <c r="F31" s="63"/>
     </row>
     <row r="32" ht="19" customHeight="1" spans="3:6">
       <c r="C32" s="28"/>
       <c r="D32" s="29"/>
-      <c r="F32" s="62"/>
+      <c r="F32" s="63"/>
     </row>
     <row r="33" ht="19" customHeight="1" spans="3:6">
       <c r="C33" s="28"/>
@@ -7149,7 +7163,7 @@
     <row r="35" ht="19" customHeight="1" spans="3:6">
       <c r="C35" s="28"/>
       <c r="D35" s="29"/>
-      <c r="F35" s="62"/>
+      <c r="F35" s="63"/>
     </row>
     <row r="36" ht="21" customHeight="1" spans="3:4">
       <c r="C36" s="28"/>
@@ -7195,11 +7209,11 @@
       <c r="H41" s="29"/>
       <c r="I41" s="29"/>
       <c r="J41" s="37"/>
-      <c r="K41" s="41"/>
-      <c r="L41" s="49"/>
-      <c r="M41" s="50"/>
-      <c r="N41" s="49"/>
-      <c r="O41" s="41"/>
+      <c r="K41" s="42"/>
+      <c r="L41" s="50"/>
+      <c r="M41" s="51"/>
+      <c r="N41" s="50"/>
+      <c r="O41" s="42"/>
     </row>
     <row r="42" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A42" s="36"/>
@@ -7212,11 +7226,11 @@
       <c r="H42" s="29"/>
       <c r="I42" s="29"/>
       <c r="J42" s="37"/>
-      <c r="K42" s="41"/>
-      <c r="L42" s="49"/>
-      <c r="M42" s="50"/>
-      <c r="N42" s="49"/>
-      <c r="O42" s="41"/>
+      <c r="K42" s="42"/>
+      <c r="L42" s="50"/>
+      <c r="M42" s="51"/>
+      <c r="N42" s="50"/>
+      <c r="O42" s="42"/>
     </row>
     <row r="43" customFormat="1" ht="29" customHeight="1" spans="1:15">
       <c r="A43" s="36"/>
@@ -7229,11 +7243,11 @@
       <c r="H43" s="29"/>
       <c r="I43" s="29"/>
       <c r="J43" s="37"/>
-      <c r="K43" s="41"/>
-      <c r="L43" s="49"/>
-      <c r="M43" s="50"/>
-      <c r="N43" s="49"/>
-      <c r="O43" s="41"/>
+      <c r="K43" s="42"/>
+      <c r="L43" s="50"/>
+      <c r="M43" s="51"/>
+      <c r="N43" s="50"/>
+      <c r="O43" s="42"/>
     </row>
     <row r="44" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A44" s="36"/>
@@ -7246,11 +7260,11 @@
       <c r="H44" s="29"/>
       <c r="I44" s="29"/>
       <c r="J44" s="37"/>
-      <c r="K44" s="41"/>
-      <c r="L44" s="49"/>
-      <c r="M44" s="50"/>
-      <c r="N44" s="49"/>
-      <c r="O44" s="41"/>
+      <c r="K44" s="42"/>
+      <c r="L44" s="50"/>
+      <c r="M44" s="51"/>
+      <c r="N44" s="50"/>
+      <c r="O44" s="42"/>
     </row>
     <row r="45" s="5" customFormat="1" ht="38" customHeight="1" spans="1:15">
       <c r="A45" s="22"/>
@@ -7259,15 +7273,15 @@
       <c r="D45" s="29"/>
       <c r="E45" s="31"/>
       <c r="F45" s="31"/>
-      <c r="G45" s="63"/>
-      <c r="H45" s="63"/>
-      <c r="I45" s="63"/>
-      <c r="J45" s="64"/>
-      <c r="K45" s="52"/>
-      <c r="L45" s="51"/>
-      <c r="M45" s="65"/>
-      <c r="N45" s="51"/>
-      <c r="O45" s="52"/>
+      <c r="G45" s="64"/>
+      <c r="H45" s="64"/>
+      <c r="I45" s="64"/>
+      <c r="J45" s="65"/>
+      <c r="K45" s="53"/>
+      <c r="L45" s="52"/>
+      <c r="M45" s="66"/>
+      <c r="N45" s="52"/>
+      <c r="O45" s="53"/>
     </row>
     <row r="46" s="5" customFormat="1" ht="25" customHeight="1" spans="1:15">
       <c r="A46" s="22"/>
@@ -7276,15 +7290,15 @@
       <c r="D46" s="31"/>
       <c r="E46" s="31"/>
       <c r="F46" s="31"/>
-      <c r="G46" s="63"/>
-      <c r="H46" s="63"/>
-      <c r="I46" s="63"/>
-      <c r="J46" s="64"/>
-      <c r="K46" s="52"/>
-      <c r="L46" s="51"/>
-      <c r="M46" s="65"/>
-      <c r="N46" s="51"/>
-      <c r="O46" s="52"/>
+      <c r="G46" s="64"/>
+      <c r="H46" s="64"/>
+      <c r="I46" s="64"/>
+      <c r="J46" s="65"/>
+      <c r="K46" s="53"/>
+      <c r="L46" s="52"/>
+      <c r="M46" s="66"/>
+      <c r="N46" s="52"/>
+      <c r="O46" s="53"/>
     </row>
     <row r="47" s="1" customFormat="1" ht="23" customHeight="1" spans="1:16">
       <c r="A47" s="36"/>
@@ -10166,7 +10180,7 @@
     </row>
     <row r="207" ht="23" customHeight="1" spans="1:15">
       <c r="A207" s="36"/>
-      <c r="B207" s="39"/>
+      <c r="B207" s="40"/>
       <c r="C207" s="28"/>
       <c r="D207" s="29"/>
       <c r="E207" s="29"/>
@@ -10175,15 +10189,15 @@
       <c r="H207" s="29"/>
       <c r="I207" s="29"/>
       <c r="J207" s="37"/>
-      <c r="K207" s="41"/>
-      <c r="L207" s="49"/>
-      <c r="M207" s="50"/>
-      <c r="N207" s="49"/>
-      <c r="O207" s="41"/>
+      <c r="K207" s="42"/>
+      <c r="L207" s="50"/>
+      <c r="M207" s="51"/>
+      <c r="N207" s="50"/>
+      <c r="O207" s="42"/>
     </row>
     <row r="208" ht="23" customHeight="1" spans="1:15">
       <c r="A208" s="36"/>
-      <c r="B208" s="39"/>
+      <c r="B208" s="40"/>
       <c r="C208" s="28"/>
       <c r="D208" s="29"/>
       <c r="E208" s="29"/>
@@ -10192,15 +10206,15 @@
       <c r="H208" s="29"/>
       <c r="I208" s="29"/>
       <c r="J208" s="37"/>
-      <c r="K208" s="41"/>
-      <c r="L208" s="49"/>
-      <c r="M208" s="50"/>
-      <c r="N208" s="49"/>
-      <c r="O208" s="41"/>
+      <c r="K208" s="42"/>
+      <c r="L208" s="50"/>
+      <c r="M208" s="51"/>
+      <c r="N208" s="50"/>
+      <c r="O208" s="42"/>
     </row>
     <row r="209" ht="23" customHeight="1" spans="1:15">
       <c r="A209" s="36"/>
-      <c r="B209" s="39"/>
+      <c r="B209" s="40"/>
       <c r="C209" s="28"/>
       <c r="D209" s="29"/>
       <c r="E209" s="29"/>
@@ -10209,15 +10223,15 @@
       <c r="H209" s="29"/>
       <c r="I209" s="29"/>
       <c r="J209" s="37"/>
-      <c r="K209" s="41"/>
-      <c r="L209" s="49"/>
-      <c r="M209" s="50"/>
-      <c r="N209" s="49"/>
-      <c r="O209" s="41"/>
+      <c r="K209" s="42"/>
+      <c r="L209" s="50"/>
+      <c r="M209" s="51"/>
+      <c r="N209" s="50"/>
+      <c r="O209" s="42"/>
     </row>
     <row r="210" ht="23" customHeight="1" spans="1:15">
       <c r="A210" s="36"/>
-      <c r="B210" s="39"/>
+      <c r="B210" s="40"/>
       <c r="C210" s="28"/>
       <c r="D210" s="29"/>
       <c r="E210" s="29"/>
@@ -10226,15 +10240,15 @@
       <c r="H210" s="29"/>
       <c r="I210" s="29"/>
       <c r="J210" s="37"/>
-      <c r="K210" s="41"/>
-      <c r="L210" s="49"/>
-      <c r="M210" s="50"/>
-      <c r="N210" s="49"/>
-      <c r="O210" s="41"/>
+      <c r="K210" s="42"/>
+      <c r="L210" s="50"/>
+      <c r="M210" s="51"/>
+      <c r="N210" s="50"/>
+      <c r="O210" s="42"/>
     </row>
     <row r="211" ht="23" customHeight="1" spans="1:15">
       <c r="A211" s="36"/>
-      <c r="B211" s="39"/>
+      <c r="B211" s="40"/>
       <c r="C211" s="28"/>
       <c r="D211" s="29"/>
       <c r="E211" s="29"/>
@@ -10243,15 +10257,15 @@
       <c r="H211" s="29"/>
       <c r="I211" s="29"/>
       <c r="J211" s="37"/>
-      <c r="K211" s="41"/>
-      <c r="L211" s="49"/>
-      <c r="M211" s="50"/>
-      <c r="N211" s="49"/>
-      <c r="O211" s="41"/>
+      <c r="K211" s="42"/>
+      <c r="L211" s="50"/>
+      <c r="M211" s="51"/>
+      <c r="N211" s="50"/>
+      <c r="O211" s="42"/>
     </row>
     <row r="212" ht="23" customHeight="1" spans="1:15">
       <c r="A212" s="36"/>
-      <c r="B212" s="39"/>
+      <c r="B212" s="40"/>
       <c r="C212" s="28"/>
       <c r="D212" s="29"/>
       <c r="E212" s="29"/>
@@ -10260,15 +10274,15 @@
       <c r="H212" s="29"/>
       <c r="I212" s="29"/>
       <c r="J212" s="37"/>
-      <c r="K212" s="41"/>
-      <c r="L212" s="49"/>
-      <c r="M212" s="50"/>
-      <c r="N212" s="49"/>
-      <c r="O212" s="41"/>
+      <c r="K212" s="42"/>
+      <c r="L212" s="50"/>
+      <c r="M212" s="51"/>
+      <c r="N212" s="50"/>
+      <c r="O212" s="42"/>
     </row>
     <row r="213" ht="23" customHeight="1" spans="1:15">
       <c r="A213" s="36"/>
-      <c r="B213" s="39"/>
+      <c r="B213" s="40"/>
       <c r="C213" s="28"/>
       <c r="D213" s="29"/>
       <c r="E213" s="29"/>
@@ -10277,15 +10291,15 @@
       <c r="H213" s="29"/>
       <c r="I213" s="29"/>
       <c r="J213" s="37"/>
-      <c r="K213" s="41"/>
-      <c r="L213" s="49"/>
-      <c r="M213" s="50"/>
-      <c r="N213" s="49"/>
-      <c r="O213" s="41"/>
+      <c r="K213" s="42"/>
+      <c r="L213" s="50"/>
+      <c r="M213" s="51"/>
+      <c r="N213" s="50"/>
+      <c r="O213" s="42"/>
     </row>
     <row r="214" ht="23" customHeight="1" spans="1:15">
       <c r="A214" s="36"/>
-      <c r="B214" s="39"/>
+      <c r="B214" s="40"/>
       <c r="C214" s="28"/>
       <c r="D214" s="29"/>
       <c r="E214" s="29"/>
@@ -10294,15 +10308,15 @@
       <c r="H214" s="29"/>
       <c r="I214" s="29"/>
       <c r="J214" s="37"/>
-      <c r="K214" s="41"/>
-      <c r="L214" s="49"/>
-      <c r="M214" s="50"/>
-      <c r="N214" s="49"/>
-      <c r="O214" s="41"/>
+      <c r="K214" s="42"/>
+      <c r="L214" s="50"/>
+      <c r="M214" s="51"/>
+      <c r="N214" s="50"/>
+      <c r="O214" s="42"/>
     </row>
     <row r="215" ht="23" customHeight="1" spans="1:15">
       <c r="A215" s="36"/>
-      <c r="B215" s="39"/>
+      <c r="B215" s="40"/>
       <c r="C215" s="28"/>
       <c r="D215" s="29"/>
       <c r="E215" s="29"/>
@@ -10311,15 +10325,15 @@
       <c r="H215" s="29"/>
       <c r="I215" s="29"/>
       <c r="J215" s="37"/>
-      <c r="K215" s="41"/>
-      <c r="L215" s="49"/>
-      <c r="M215" s="50"/>
-      <c r="N215" s="49"/>
-      <c r="O215" s="41"/>
+      <c r="K215" s="42"/>
+      <c r="L215" s="50"/>
+      <c r="M215" s="51"/>
+      <c r="N215" s="50"/>
+      <c r="O215" s="42"/>
     </row>
     <row r="216" ht="23" customHeight="1" spans="1:15">
       <c r="A216" s="36"/>
-      <c r="B216" s="39"/>
+      <c r="B216" s="40"/>
       <c r="C216" s="28"/>
       <c r="D216" s="29"/>
       <c r="E216" s="29"/>
@@ -10328,15 +10342,15 @@
       <c r="H216" s="29"/>
       <c r="I216" s="29"/>
       <c r="J216" s="37"/>
-      <c r="K216" s="41"/>
-      <c r="L216" s="49"/>
-      <c r="M216" s="50"/>
-      <c r="N216" s="49"/>
-      <c r="O216" s="41"/>
+      <c r="K216" s="42"/>
+      <c r="L216" s="50"/>
+      <c r="M216" s="51"/>
+      <c r="N216" s="50"/>
+      <c r="O216" s="42"/>
     </row>
     <row r="217" ht="23" customHeight="1" spans="1:15">
       <c r="A217" s="36"/>
-      <c r="B217" s="39"/>
+      <c r="B217" s="40"/>
       <c r="C217" s="28"/>
       <c r="D217" s="29"/>
       <c r="E217" s="29"/>
@@ -10345,15 +10359,15 @@
       <c r="H217" s="29"/>
       <c r="I217" s="29"/>
       <c r="J217" s="37"/>
-      <c r="K217" s="41"/>
-      <c r="L217" s="49"/>
-      <c r="M217" s="50"/>
-      <c r="N217" s="49"/>
-      <c r="O217" s="41"/>
+      <c r="K217" s="42"/>
+      <c r="L217" s="50"/>
+      <c r="M217" s="51"/>
+      <c r="N217" s="50"/>
+      <c r="O217" s="42"/>
     </row>
     <row r="218" ht="23" customHeight="1" spans="1:15">
       <c r="A218" s="36"/>
-      <c r="B218" s="39"/>
+      <c r="B218" s="40"/>
       <c r="C218" s="28"/>
       <c r="D218" s="29"/>
       <c r="E218" s="29"/>
@@ -10362,15 +10376,15 @@
       <c r="H218" s="29"/>
       <c r="I218" s="29"/>
       <c r="J218" s="37"/>
-      <c r="K218" s="41"/>
-      <c r="L218" s="49"/>
-      <c r="M218" s="50"/>
-      <c r="N218" s="49"/>
-      <c r="O218" s="41"/>
+      <c r="K218" s="42"/>
+      <c r="L218" s="50"/>
+      <c r="M218" s="51"/>
+      <c r="N218" s="50"/>
+      <c r="O218" s="42"/>
     </row>
     <row r="219" ht="23" customHeight="1" spans="1:15">
       <c r="A219" s="36"/>
-      <c r="B219" s="39"/>
+      <c r="B219" s="40"/>
       <c r="C219" s="28"/>
       <c r="D219" s="29"/>
       <c r="E219" s="29"/>
@@ -10379,15 +10393,15 @@
       <c r="H219" s="29"/>
       <c r="I219" s="29"/>
       <c r="J219" s="37"/>
-      <c r="K219" s="41"/>
-      <c r="L219" s="49"/>
-      <c r="M219" s="50"/>
-      <c r="N219" s="49"/>
-      <c r="O219" s="41"/>
+      <c r="K219" s="42"/>
+      <c r="L219" s="50"/>
+      <c r="M219" s="51"/>
+      <c r="N219" s="50"/>
+      <c r="O219" s="42"/>
     </row>
     <row r="220" ht="23" customHeight="1" spans="1:15">
       <c r="A220" s="36"/>
-      <c r="B220" s="39"/>
+      <c r="B220" s="40"/>
       <c r="C220" s="28"/>
       <c r="D220" s="29"/>
       <c r="E220" s="29"/>
@@ -10396,15 +10410,15 @@
       <c r="H220" s="29"/>
       <c r="I220" s="29"/>
       <c r="J220" s="37"/>
-      <c r="K220" s="41"/>
-      <c r="L220" s="49"/>
-      <c r="M220" s="50"/>
-      <c r="N220" s="49"/>
-      <c r="O220" s="41"/>
+      <c r="K220" s="42"/>
+      <c r="L220" s="50"/>
+      <c r="M220" s="51"/>
+      <c r="N220" s="50"/>
+      <c r="O220" s="42"/>
     </row>
     <row r="221" ht="23" customHeight="1" spans="1:15">
       <c r="A221" s="36"/>
-      <c r="B221" s="39"/>
+      <c r="B221" s="40"/>
       <c r="C221" s="28"/>
       <c r="D221" s="29"/>
       <c r="E221" s="29"/>
@@ -10413,15 +10427,15 @@
       <c r="H221" s="29"/>
       <c r="I221" s="29"/>
       <c r="J221" s="37"/>
-      <c r="K221" s="41"/>
-      <c r="L221" s="49"/>
-      <c r="M221" s="50"/>
-      <c r="N221" s="49"/>
-      <c r="O221" s="41"/>
+      <c r="K221" s="42"/>
+      <c r="L221" s="50"/>
+      <c r="M221" s="51"/>
+      <c r="N221" s="50"/>
+      <c r="O221" s="42"/>
     </row>
     <row r="222" ht="23" customHeight="1" spans="1:15">
       <c r="A222" s="36"/>
-      <c r="B222" s="39"/>
+      <c r="B222" s="40"/>
       <c r="C222" s="28"/>
       <c r="D222" s="29"/>
       <c r="E222" s="29"/>
@@ -10430,15 +10444,15 @@
       <c r="H222" s="29"/>
       <c r="I222" s="29"/>
       <c r="J222" s="37"/>
-      <c r="K222" s="41"/>
-      <c r="L222" s="49"/>
-      <c r="M222" s="50"/>
-      <c r="N222" s="49"/>
-      <c r="O222" s="41"/>
+      <c r="K222" s="42"/>
+      <c r="L222" s="50"/>
+      <c r="M222" s="51"/>
+      <c r="N222" s="50"/>
+      <c r="O222" s="42"/>
     </row>
     <row r="223" ht="23" customHeight="1" spans="1:15">
       <c r="A223" s="36"/>
-      <c r="B223" s="39"/>
+      <c r="B223" s="40"/>
       <c r="C223" s="28"/>
       <c r="D223" s="29"/>
       <c r="E223" s="29"/>
@@ -10447,15 +10461,15 @@
       <c r="H223" s="29"/>
       <c r="I223" s="29"/>
       <c r="J223" s="37"/>
-      <c r="K223" s="41"/>
-      <c r="L223" s="49"/>
-      <c r="M223" s="50"/>
-      <c r="N223" s="49"/>
-      <c r="O223" s="41"/>
+      <c r="K223" s="42"/>
+      <c r="L223" s="50"/>
+      <c r="M223" s="51"/>
+      <c r="N223" s="50"/>
+      <c r="O223" s="42"/>
     </row>
     <row r="224" ht="23" customHeight="1" spans="1:15">
       <c r="A224" s="36"/>
-      <c r="B224" s="39"/>
+      <c r="B224" s="40"/>
       <c r="C224" s="28"/>
       <c r="D224" s="29"/>
       <c r="E224" s="29"/>
@@ -10464,15 +10478,15 @@
       <c r="H224" s="29"/>
       <c r="I224" s="29"/>
       <c r="J224" s="37"/>
-      <c r="K224" s="41"/>
-      <c r="L224" s="49"/>
-      <c r="M224" s="50"/>
-      <c r="N224" s="49"/>
-      <c r="O224" s="41"/>
+      <c r="K224" s="42"/>
+      <c r="L224" s="50"/>
+      <c r="M224" s="51"/>
+      <c r="N224" s="50"/>
+      <c r="O224" s="42"/>
     </row>
     <row r="225" ht="23" customHeight="1" spans="1:15">
       <c r="A225" s="36"/>
-      <c r="B225" s="39"/>
+      <c r="B225" s="40"/>
       <c r="C225" s="28"/>
       <c r="D225" s="29"/>
       <c r="E225" s="29"/>
@@ -10481,11 +10495,11 @@
       <c r="H225" s="29"/>
       <c r="I225" s="29"/>
       <c r="J225" s="37"/>
-      <c r="K225" s="41"/>
-      <c r="L225" s="49"/>
-      <c r="M225" s="50"/>
-      <c r="N225" s="49"/>
-      <c r="O225" s="41"/>
+      <c r="K225" s="42"/>
+      <c r="L225" s="50"/>
+      <c r="M225" s="51"/>
+      <c r="N225" s="50"/>
+      <c r="O225" s="42"/>
     </row>
   </sheetData>
   <sheetProtection insertRows="0" insertHyperlinks="0" deleteRows="0"/>
@@ -10601,13 +10615,13 @@
   <sheetPr/>
   <dimension ref="A1:P299"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="44.5333333333333" style="6" customWidth="1"/>
     <col min="2" max="2" width="42.75" style="7" customWidth="1"/>
@@ -10626,7 +10640,7 @@
     <col min="16" max="16384" width="10.8333333333333" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.15" spans="1:15">
+    <row r="1" ht="15.25" spans="1:15">
       <c r="A1" s="15" t="s">
         <v>725</v>
       </c>
@@ -10648,16 +10662,16 @@
       <c r="I1" s="17" t="s">
         <v>730</v>
       </c>
-      <c r="J1" s="40"/>
-      <c r="K1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="42"/>
       <c r="L1" s="17" t="s">
         <v>731</v>
       </c>
       <c r="M1" s="17"/>
       <c r="N1" s="17"/>
-      <c r="O1" s="42"/>
-    </row>
-    <row r="2" s="1" customFormat="1" ht="15.15" spans="1:15">
+      <c r="O1" s="43"/>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="18" t="s">
         <v>753</v>
       </c>
@@ -10669,12 +10683,12 @@
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
       <c r="I2" s="21"/>
-      <c r="J2" s="43"/>
+      <c r="J2" s="44"/>
       <c r="K2" s="25"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
     </row>
     <row r="3" s="1" customFormat="1" ht="10" customHeight="1" spans="1:15">
       <c r="A3" s="22"/>
@@ -10686,7 +10700,7 @@
       <c r="G3" s="26"/>
       <c r="H3" s="26"/>
       <c r="I3" s="26"/>
-      <c r="J3" s="46"/>
+      <c r="J3" s="47"/>
       <c r="K3" s="25"/>
       <c r="L3" s="26"/>
       <c r="M3" s="24"/>
@@ -10721,10 +10735,10 @@
       <c r="I4" s="27" t="s">
         <v>740</v>
       </c>
-      <c r="J4" s="47" t="s">
+      <c r="J4" s="48" t="s">
         <v>741</v>
       </c>
-      <c r="K4" s="48"/>
+      <c r="K4" s="49"/>
       <c r="L4" s="27" t="s">
         <v>742</v>
       </c>
@@ -11178,11 +11192,11 @@
       <c r="H21" s="29"/>
       <c r="I21" s="29"/>
       <c r="J21" s="37"/>
-      <c r="K21" s="41"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="50"/>
-      <c r="N21" s="49"/>
-      <c r="O21" s="41"/>
+      <c r="K21" s="42"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="50"/>
+      <c r="O21" s="42"/>
     </row>
     <row r="22" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A22" s="36" t="s">
@@ -11205,11 +11219,11 @@
       <c r="H22" s="29"/>
       <c r="I22" s="29"/>
       <c r="J22" s="37"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="50"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="41"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="51"/>
+      <c r="N22" s="50"/>
+      <c r="O22" s="42"/>
     </row>
     <row r="23" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A23" s="36"/>
@@ -11230,11 +11244,11 @@
       <c r="H23" s="29"/>
       <c r="I23" s="29"/>
       <c r="J23" s="37"/>
-      <c r="K23" s="41"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="49"/>
-      <c r="O23" s="41"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="51"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="42"/>
     </row>
     <row r="24" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A24" s="36"/>
@@ -11257,11 +11271,11 @@
       <c r="H24" s="29"/>
       <c r="I24" s="29"/>
       <c r="J24" s="37"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="50"/>
-      <c r="N24" s="49"/>
-      <c r="O24" s="41"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="50"/>
+      <c r="M24" s="51"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="42"/>
     </row>
     <row r="25" s="4" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A25" s="36"/>
@@ -11282,11 +11296,11 @@
       <c r="H25" s="29"/>
       <c r="I25" s="29"/>
       <c r="J25" s="37"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="50"/>
-      <c r="N25" s="49"/>
-      <c r="O25" s="41"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="50"/>
+      <c r="M25" s="51"/>
+      <c r="N25" s="50"/>
+      <c r="O25" s="42"/>
     </row>
     <row r="26" ht="22" customHeight="1" spans="2:6">
       <c r="B26" s="23" t="s">
@@ -11378,11 +11392,11 @@
       <c r="H29" s="29"/>
       <c r="I29" s="29"/>
       <c r="J29" s="37"/>
-      <c r="K29" s="41"/>
-      <c r="L29" s="49"/>
-      <c r="M29" s="50"/>
-      <c r="N29" s="49"/>
-      <c r="O29" s="41"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="51"/>
+      <c r="N29" s="50"/>
+      <c r="O29" s="42"/>
     </row>
     <row r="30" customFormat="1" ht="33" customHeight="1" spans="1:15">
       <c r="A30" s="36"/>
@@ -11405,11 +11419,11 @@
       <c r="H30" s="29"/>
       <c r="I30" s="29"/>
       <c r="J30" s="37"/>
-      <c r="K30" s="41"/>
-      <c r="L30" s="49"/>
-      <c r="M30" s="50"/>
-      <c r="N30" s="49"/>
-      <c r="O30" s="41"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="51"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="42"/>
     </row>
     <row r="31" customFormat="1" ht="29" customHeight="1" spans="1:15">
       <c r="A31" s="36"/>
@@ -11430,11 +11444,11 @@
       <c r="H31" s="29"/>
       <c r="I31" s="29"/>
       <c r="J31" s="37"/>
-      <c r="K31" s="41"/>
-      <c r="L31" s="49"/>
-      <c r="M31" s="50"/>
-      <c r="N31" s="49"/>
-      <c r="O31" s="41"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="50"/>
+      <c r="M31" s="51"/>
+      <c r="N31" s="50"/>
+      <c r="O31" s="42"/>
     </row>
     <row r="32" customFormat="1" ht="29" customHeight="1" spans="1:15">
       <c r="A32" s="36"/>
@@ -11455,11 +11469,11 @@
       <c r="H32" s="29"/>
       <c r="I32" s="29"/>
       <c r="J32" s="37"/>
-      <c r="K32" s="41"/>
-      <c r="L32" s="49"/>
-      <c r="M32" s="50"/>
-      <c r="N32" s="49"/>
-      <c r="O32" s="41"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="50"/>
+      <c r="M32" s="51"/>
+      <c r="N32" s="50"/>
+      <c r="O32" s="42"/>
     </row>
     <row r="33" customFormat="1" ht="29" customHeight="1" spans="1:15">
       <c r="A33" s="36"/>
@@ -11482,14 +11496,16 @@
       <c r="H33" s="29"/>
       <c r="I33" s="29"/>
       <c r="J33" s="37"/>
-      <c r="K33" s="41"/>
-      <c r="L33" s="49"/>
-      <c r="M33" s="50"/>
-      <c r="N33" s="49"/>
-      <c r="O33" s="41"/>
+      <c r="K33" s="42"/>
+      <c r="L33" s="50"/>
+      <c r="M33" s="51"/>
+      <c r="N33" s="50"/>
+      <c r="O33" s="42"/>
     </row>
     <row r="34" customFormat="1" ht="29" customHeight="1" spans="1:15">
-      <c r="A34" s="36"/>
+      <c r="A34" s="39" t="s">
+        <v>825</v>
+      </c>
       <c r="B34" s="23"/>
       <c r="C34" s="28"/>
       <c r="D34" s="29"/>
@@ -11499,11 +11515,11 @@
       <c r="H34" s="29"/>
       <c r="I34" s="29"/>
       <c r="J34" s="37"/>
-      <c r="K34" s="41"/>
-      <c r="L34" s="49"/>
-      <c r="M34" s="50"/>
-      <c r="N34" s="49"/>
-      <c r="O34" s="41"/>
+      <c r="K34" s="42"/>
+      <c r="L34" s="50"/>
+      <c r="M34" s="51"/>
+      <c r="N34" s="50"/>
+      <c r="O34" s="42"/>
     </row>
     <row r="35" customFormat="1" ht="29" customHeight="1" spans="1:15">
       <c r="A35" s="36"/>
@@ -11516,11 +11532,11 @@
       <c r="H35" s="29"/>
       <c r="I35" s="29"/>
       <c r="J35" s="37"/>
-      <c r="K35" s="41"/>
-      <c r="L35" s="49"/>
-      <c r="M35" s="50"/>
-      <c r="N35" s="49"/>
-      <c r="O35" s="41"/>
+      <c r="K35" s="42"/>
+      <c r="L35" s="50"/>
+      <c r="M35" s="51"/>
+      <c r="N35" s="50"/>
+      <c r="O35" s="42"/>
     </row>
     <row r="36" customFormat="1" ht="29" customHeight="1" spans="1:15">
       <c r="A36" s="36"/>
@@ -11533,11 +11549,11 @@
       <c r="H36" s="29"/>
       <c r="I36" s="29"/>
       <c r="J36" s="37"/>
-      <c r="K36" s="41"/>
-      <c r="L36" s="49"/>
-      <c r="M36" s="50"/>
-      <c r="N36" s="49"/>
-      <c r="O36" s="41"/>
+      <c r="K36" s="42"/>
+      <c r="L36" s="50"/>
+      <c r="M36" s="51"/>
+      <c r="N36" s="50"/>
+      <c r="O36" s="42"/>
     </row>
     <row r="37" customFormat="1" ht="29" customHeight="1" spans="1:15">
       <c r="A37" s="36"/>
@@ -11550,11 +11566,11 @@
       <c r="H37" s="29"/>
       <c r="I37" s="29"/>
       <c r="J37" s="37"/>
-      <c r="K37" s="41"/>
-      <c r="L37" s="49"/>
-      <c r="M37" s="50"/>
-      <c r="N37" s="49"/>
-      <c r="O37" s="41"/>
+      <c r="K37" s="42"/>
+      <c r="L37" s="50"/>
+      <c r="M37" s="51"/>
+      <c r="N37" s="50"/>
+      <c r="O37" s="42"/>
     </row>
     <row r="38" customFormat="1" ht="29" customHeight="1" spans="1:15">
       <c r="A38" s="36"/>
@@ -11567,11 +11583,11 @@
       <c r="H38" s="29"/>
       <c r="I38" s="29"/>
       <c r="J38" s="37"/>
-      <c r="K38" s="41"/>
-      <c r="L38" s="49"/>
-      <c r="M38" s="50"/>
-      <c r="N38" s="49"/>
-      <c r="O38" s="41"/>
+      <c r="K38" s="42"/>
+      <c r="L38" s="50"/>
+      <c r="M38" s="51"/>
+      <c r="N38" s="50"/>
+      <c r="O38" s="42"/>
     </row>
     <row r="39" customFormat="1" ht="29" customHeight="1" spans="1:15">
       <c r="A39" s="36"/>
@@ -11584,11 +11600,11 @@
       <c r="H39" s="29"/>
       <c r="I39" s="29"/>
       <c r="J39" s="37"/>
-      <c r="K39" s="41"/>
-      <c r="L39" s="49"/>
-      <c r="M39" s="50"/>
-      <c r="N39" s="49"/>
-      <c r="O39" s="41"/>
+      <c r="K39" s="42"/>
+      <c r="L39" s="50"/>
+      <c r="M39" s="51"/>
+      <c r="N39" s="50"/>
+      <c r="O39" s="42"/>
     </row>
     <row r="40" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A40" s="36"/>
@@ -11601,11 +11617,11 @@
       <c r="H40" s="29"/>
       <c r="I40" s="29"/>
       <c r="J40" s="37"/>
-      <c r="K40" s="41"/>
-      <c r="L40" s="49"/>
-      <c r="M40" s="50"/>
-      <c r="N40" s="49"/>
-      <c r="O40" s="41"/>
+      <c r="K40" s="42"/>
+      <c r="L40" s="50"/>
+      <c r="M40" s="51"/>
+      <c r="N40" s="50"/>
+      <c r="O40" s="42"/>
     </row>
     <row r="41" s="5" customFormat="1" ht="25" customHeight="1" spans="1:15">
       <c r="A41" s="22"/>
@@ -11621,8 +11637,8 @@
       <c r="K41" s="25"/>
       <c r="L41" s="26"/>
       <c r="M41" s="24"/>
-      <c r="N41" s="51"/>
-      <c r="O41" s="52"/>
+      <c r="N41" s="52"/>
+      <c r="O41" s="53"/>
     </row>
     <row r="42" s="5" customFormat="1" ht="25" customHeight="1" spans="1:15">
       <c r="A42" s="22"/>
@@ -11638,12 +11654,12 @@
       <c r="K42" s="25"/>
       <c r="L42" s="26"/>
       <c r="M42" s="24"/>
-      <c r="N42" s="51"/>
-      <c r="O42" s="52"/>
+      <c r="N42" s="52"/>
+      <c r="O42" s="53"/>
     </row>
     <row r="43" s="5" customFormat="1" ht="25" customHeight="1" spans="1:15">
       <c r="A43" s="22"/>
-      <c r="B43" s="39"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="35"/>
       <c r="D43" s="31"/>
       <c r="E43" s="31"/>
@@ -11655,8 +11671,8 @@
       <c r="K43" s="25"/>
       <c r="L43" s="26"/>
       <c r="M43" s="24"/>
-      <c r="N43" s="51"/>
-      <c r="O43" s="52"/>
+      <c r="N43" s="52"/>
+      <c r="O43" s="53"/>
     </row>
     <row r="44" s="1" customFormat="1" ht="23" customHeight="1" spans="1:16">
       <c r="A44" s="36"/>
@@ -12427,9 +12443,9 @@
       <c r="K86" s="4"/>
       <c r="L86" s="4"/>
       <c r="M86" s="4"/>
-      <c r="N86" s="53"/>
-      <c r="O86" s="53"/>
-      <c r="P86" s="53"/>
+      <c r="N86" s="54"/>
+      <c r="O86" s="54"/>
+      <c r="P86" s="54"/>
     </row>
     <row r="87" ht="34" customHeight="1" spans="1:16">
       <c r="A87" s="22"/>
@@ -12445,9 +12461,9 @@
       <c r="K87" s="4"/>
       <c r="L87" s="4"/>
       <c r="M87" s="4"/>
-      <c r="N87" s="53"/>
-      <c r="O87" s="53"/>
-      <c r="P87" s="53"/>
+      <c r="N87" s="54"/>
+      <c r="O87" s="54"/>
+      <c r="P87" s="54"/>
     </row>
     <row r="88" ht="34" customHeight="1" spans="1:16">
       <c r="A88" s="22"/>
@@ -12463,9 +12479,9 @@
       <c r="K88" s="4"/>
       <c r="L88" s="4"/>
       <c r="M88" s="4"/>
-      <c r="N88" s="53"/>
-      <c r="O88" s="53"/>
-      <c r="P88" s="53"/>
+      <c r="N88" s="54"/>
+      <c r="O88" s="54"/>
+      <c r="P88" s="54"/>
     </row>
     <row r="89" ht="34" customHeight="1" spans="1:16">
       <c r="A89" s="22"/>
@@ -12481,9 +12497,9 @@
       <c r="K89" s="4"/>
       <c r="L89" s="4"/>
       <c r="M89" s="4"/>
-      <c r="N89" s="53"/>
-      <c r="O89" s="53"/>
-      <c r="P89" s="53"/>
+      <c r="N89" s="54"/>
+      <c r="O89" s="54"/>
+      <c r="P89" s="54"/>
     </row>
     <row r="90" ht="34" customHeight="1" spans="1:16">
       <c r="A90" s="36"/>
@@ -12496,12 +12512,12 @@
       <c r="H90" s="29"/>
       <c r="I90" s="29"/>
       <c r="J90" s="37"/>
-      <c r="K90" s="41"/>
-      <c r="L90" s="49"/>
-      <c r="M90" s="50"/>
-      <c r="N90" s="54"/>
-      <c r="O90" s="55"/>
-      <c r="P90" s="53"/>
+      <c r="K90" s="42"/>
+      <c r="L90" s="50"/>
+      <c r="M90" s="51"/>
+      <c r="N90" s="55"/>
+      <c r="O90" s="56"/>
+      <c r="P90" s="54"/>
     </row>
     <row r="91" ht="34" customHeight="1" spans="1:16">
       <c r="A91" s="36"/>
@@ -12514,12 +12530,12 @@
       <c r="H91" s="29"/>
       <c r="I91" s="29"/>
       <c r="J91" s="37"/>
-      <c r="K91" s="41"/>
-      <c r="L91" s="49"/>
-      <c r="M91" s="50"/>
-      <c r="N91" s="54"/>
-      <c r="O91" s="55"/>
-      <c r="P91" s="53"/>
+      <c r="K91" s="42"/>
+      <c r="L91" s="50"/>
+      <c r="M91" s="51"/>
+      <c r="N91" s="55"/>
+      <c r="O91" s="56"/>
+      <c r="P91" s="54"/>
     </row>
     <row r="92" ht="34" customHeight="1" spans="1:16">
       <c r="A92" s="22"/>
@@ -12535,8 +12551,8 @@
       <c r="K92" s="25"/>
       <c r="L92" s="26"/>
       <c r="M92" s="24"/>
-      <c r="N92" s="51"/>
-      <c r="O92" s="52"/>
+      <c r="N92" s="52"/>
+      <c r="O92" s="53"/>
       <c r="P92" s="5"/>
     </row>
     <row r="93" ht="34" customHeight="1" spans="1:16">
@@ -12553,8 +12569,8 @@
       <c r="K93" s="25"/>
       <c r="L93" s="26"/>
       <c r="M93" s="24"/>
-      <c r="N93" s="51"/>
-      <c r="O93" s="52"/>
+      <c r="N93" s="52"/>
+      <c r="O93" s="53"/>
       <c r="P93" s="5"/>
     </row>
     <row r="94" ht="34" customHeight="1" spans="1:16">
@@ -12571,8 +12587,8 @@
       <c r="K94" s="25"/>
       <c r="L94" s="26"/>
       <c r="M94" s="24"/>
-      <c r="N94" s="51"/>
-      <c r="O94" s="52"/>
+      <c r="N94" s="52"/>
+      <c r="O94" s="53"/>
       <c r="P94" s="5"/>
     </row>
     <row r="95" ht="34" customHeight="1" spans="1:16">
@@ -12586,12 +12602,12 @@
       <c r="H95" s="29"/>
       <c r="I95" s="29"/>
       <c r="J95" s="37"/>
-      <c r="K95" s="41"/>
-      <c r="L95" s="49"/>
-      <c r="M95" s="50"/>
-      <c r="N95" s="54"/>
-      <c r="O95" s="55"/>
-      <c r="P95" s="56"/>
+      <c r="K95" s="42"/>
+      <c r="L95" s="50"/>
+      <c r="M95" s="51"/>
+      <c r="N95" s="55"/>
+      <c r="O95" s="56"/>
+      <c r="P95" s="57"/>
     </row>
     <row r="96" ht="34" customHeight="1" spans="1:16">
       <c r="A96" s="36"/>
@@ -12604,12 +12620,12 @@
       <c r="H96" s="29"/>
       <c r="I96" s="29"/>
       <c r="J96" s="37"/>
-      <c r="K96" s="41"/>
-      <c r="L96" s="49"/>
-      <c r="M96" s="50"/>
-      <c r="N96" s="54"/>
-      <c r="O96" s="55"/>
-      <c r="P96" s="56"/>
+      <c r="K96" s="42"/>
+      <c r="L96" s="50"/>
+      <c r="M96" s="51"/>
+      <c r="N96" s="55"/>
+      <c r="O96" s="56"/>
+      <c r="P96" s="57"/>
     </row>
     <row r="97" ht="34" customHeight="1" spans="1:16">
       <c r="A97" s="36"/>
@@ -12622,12 +12638,12 @@
       <c r="H97" s="29"/>
       <c r="I97" s="29"/>
       <c r="J97" s="37"/>
-      <c r="K97" s="41"/>
-      <c r="L97" s="49"/>
-      <c r="M97" s="50"/>
-      <c r="N97" s="54"/>
-      <c r="O97" s="55"/>
-      <c r="P97" s="56"/>
+      <c r="K97" s="42"/>
+      <c r="L97" s="50"/>
+      <c r="M97" s="51"/>
+      <c r="N97" s="55"/>
+      <c r="O97" s="56"/>
+      <c r="P97" s="57"/>
     </row>
     <row r="98" ht="34" customHeight="1" spans="1:16">
       <c r="A98" s="36"/>
@@ -12640,12 +12656,12 @@
       <c r="H98" s="29"/>
       <c r="I98" s="29"/>
       <c r="J98" s="37"/>
-      <c r="K98" s="41"/>
-      <c r="L98" s="49"/>
-      <c r="M98" s="50"/>
-      <c r="N98" s="54"/>
-      <c r="O98" s="55"/>
-      <c r="P98" s="56"/>
+      <c r="K98" s="42"/>
+      <c r="L98" s="50"/>
+      <c r="M98" s="51"/>
+      <c r="N98" s="55"/>
+      <c r="O98" s="56"/>
+      <c r="P98" s="57"/>
     </row>
     <row r="99" ht="34" customHeight="1" spans="1:16">
       <c r="A99" s="36"/>
@@ -12658,12 +12674,12 @@
       <c r="H99" s="29"/>
       <c r="I99" s="29"/>
       <c r="J99" s="37"/>
-      <c r="K99" s="41"/>
-      <c r="L99" s="49"/>
-      <c r="M99" s="50"/>
-      <c r="N99" s="54"/>
-      <c r="O99" s="55"/>
-      <c r="P99" s="56"/>
+      <c r="K99" s="42"/>
+      <c r="L99" s="50"/>
+      <c r="M99" s="51"/>
+      <c r="N99" s="55"/>
+      <c r="O99" s="56"/>
+      <c r="P99" s="57"/>
     </row>
     <row r="100" ht="34" customHeight="1" spans="1:16">
       <c r="A100" s="36"/>
@@ -12676,12 +12692,12 @@
       <c r="H100" s="29"/>
       <c r="I100" s="29"/>
       <c r="J100" s="37"/>
-      <c r="K100" s="41"/>
-      <c r="L100" s="49"/>
-      <c r="M100" s="50"/>
-      <c r="N100" s="54"/>
-      <c r="O100" s="55"/>
-      <c r="P100" s="56"/>
+      <c r="K100" s="42"/>
+      <c r="L100" s="50"/>
+      <c r="M100" s="51"/>
+      <c r="N100" s="55"/>
+      <c r="O100" s="56"/>
+      <c r="P100" s="57"/>
     </row>
     <row r="101" ht="34" customHeight="1" spans="1:16">
       <c r="A101" s="36"/>
@@ -12694,12 +12710,12 @@
       <c r="H101" s="29"/>
       <c r="I101" s="29"/>
       <c r="J101" s="37"/>
-      <c r="K101" s="41"/>
-      <c r="L101" s="49"/>
-      <c r="M101" s="50"/>
-      <c r="N101" s="54"/>
-      <c r="O101" s="55"/>
-      <c r="P101" s="56"/>
+      <c r="K101" s="42"/>
+      <c r="L101" s="50"/>
+      <c r="M101" s="51"/>
+      <c r="N101" s="55"/>
+      <c r="O101" s="56"/>
+      <c r="P101" s="57"/>
     </row>
     <row r="102" ht="34" customHeight="1" spans="1:16">
       <c r="A102" s="36"/>
@@ -12712,12 +12728,12 @@
       <c r="H102" s="29"/>
       <c r="I102" s="29"/>
       <c r="J102" s="37"/>
-      <c r="K102" s="41"/>
-      <c r="L102" s="49"/>
-      <c r="M102" s="50"/>
-      <c r="N102" s="54"/>
-      <c r="O102" s="55"/>
-      <c r="P102" s="56"/>
+      <c r="K102" s="42"/>
+      <c r="L102" s="50"/>
+      <c r="M102" s="51"/>
+      <c r="N102" s="55"/>
+      <c r="O102" s="56"/>
+      <c r="P102" s="57"/>
     </row>
     <row r="103" ht="34" customHeight="1" spans="1:16">
       <c r="A103" s="36"/>
@@ -12730,12 +12746,12 @@
       <c r="H103" s="29"/>
       <c r="I103" s="29"/>
       <c r="J103" s="37"/>
-      <c r="K103" s="41"/>
-      <c r="L103" s="49"/>
-      <c r="M103" s="50"/>
-      <c r="N103" s="54"/>
-      <c r="O103" s="55"/>
-      <c r="P103" s="56"/>
+      <c r="K103" s="42"/>
+      <c r="L103" s="50"/>
+      <c r="M103" s="51"/>
+      <c r="N103" s="55"/>
+      <c r="O103" s="56"/>
+      <c r="P103" s="57"/>
     </row>
     <row r="104" ht="34" customHeight="1" spans="1:16">
       <c r="A104" s="36"/>
@@ -12748,12 +12764,12 @@
       <c r="H104" s="29"/>
       <c r="I104" s="29"/>
       <c r="J104" s="37"/>
-      <c r="K104" s="41"/>
-      <c r="L104" s="49"/>
-      <c r="M104" s="50"/>
-      <c r="N104" s="54"/>
-      <c r="O104" s="55"/>
-      <c r="P104" s="56"/>
+      <c r="K104" s="42"/>
+      <c r="L104" s="50"/>
+      <c r="M104" s="51"/>
+      <c r="N104" s="55"/>
+      <c r="O104" s="56"/>
+      <c r="P104" s="57"/>
     </row>
     <row r="105" ht="34" customHeight="1" spans="1:16">
       <c r="A105" s="36"/>
@@ -12766,12 +12782,12 @@
       <c r="H105" s="29"/>
       <c r="I105" s="29"/>
       <c r="J105" s="37"/>
-      <c r="K105" s="41"/>
-      <c r="L105" s="49"/>
-      <c r="M105" s="50"/>
-      <c r="N105" s="54"/>
-      <c r="O105" s="55"/>
-      <c r="P105" s="56"/>
+      <c r="K105" s="42"/>
+      <c r="L105" s="50"/>
+      <c r="M105" s="51"/>
+      <c r="N105" s="55"/>
+      <c r="O105" s="56"/>
+      <c r="P105" s="57"/>
     </row>
     <row r="106" ht="34" customHeight="1" spans="1:16">
       <c r="A106" s="36"/>
@@ -12784,12 +12800,12 @@
       <c r="H106" s="29"/>
       <c r="I106" s="29"/>
       <c r="J106" s="37"/>
-      <c r="K106" s="41"/>
-      <c r="L106" s="49"/>
-      <c r="M106" s="50"/>
-      <c r="N106" s="54"/>
-      <c r="O106" s="55"/>
-      <c r="P106" s="56"/>
+      <c r="K106" s="42"/>
+      <c r="L106" s="50"/>
+      <c r="M106" s="51"/>
+      <c r="N106" s="55"/>
+      <c r="O106" s="56"/>
+      <c r="P106" s="57"/>
     </row>
     <row r="107" ht="34" customHeight="1" spans="1:16">
       <c r="A107" s="36"/>
@@ -12802,12 +12818,12 @@
       <c r="H107" s="29"/>
       <c r="I107" s="29"/>
       <c r="J107" s="37"/>
-      <c r="K107" s="41"/>
-      <c r="L107" s="49"/>
-      <c r="M107" s="50"/>
-      <c r="N107" s="54"/>
-      <c r="O107" s="55"/>
-      <c r="P107" s="56"/>
+      <c r="K107" s="42"/>
+      <c r="L107" s="50"/>
+      <c r="M107" s="51"/>
+      <c r="N107" s="55"/>
+      <c r="O107" s="56"/>
+      <c r="P107" s="57"/>
     </row>
     <row r="108" ht="34" customHeight="1" spans="1:16">
       <c r="A108" s="36"/>
@@ -12820,12 +12836,12 @@
       <c r="H108" s="29"/>
       <c r="I108" s="29"/>
       <c r="J108" s="37"/>
-      <c r="K108" s="41"/>
-      <c r="L108" s="49"/>
-      <c r="M108" s="50"/>
-      <c r="N108" s="54"/>
-      <c r="O108" s="55"/>
-      <c r="P108" s="56"/>
+      <c r="K108" s="42"/>
+      <c r="L108" s="50"/>
+      <c r="M108" s="51"/>
+      <c r="N108" s="55"/>
+      <c r="O108" s="56"/>
+      <c r="P108" s="57"/>
     </row>
     <row r="109" ht="34" customHeight="1" spans="1:16">
       <c r="A109" s="36"/>
@@ -12838,12 +12854,12 @@
       <c r="H109" s="29"/>
       <c r="I109" s="29"/>
       <c r="J109" s="37"/>
-      <c r="K109" s="41"/>
-      <c r="L109" s="49"/>
-      <c r="M109" s="50"/>
-      <c r="N109" s="54"/>
-      <c r="O109" s="55"/>
-      <c r="P109" s="56"/>
+      <c r="K109" s="42"/>
+      <c r="L109" s="50"/>
+      <c r="M109" s="51"/>
+      <c r="N109" s="55"/>
+      <c r="O109" s="56"/>
+      <c r="P109" s="57"/>
     </row>
     <row r="110" ht="34" customHeight="1" spans="1:16">
       <c r="A110" s="36"/>
@@ -12856,12 +12872,12 @@
       <c r="H110" s="29"/>
       <c r="I110" s="29"/>
       <c r="J110" s="37"/>
-      <c r="K110" s="41"/>
-      <c r="L110" s="49"/>
-      <c r="M110" s="50"/>
-      <c r="N110" s="54"/>
-      <c r="O110" s="55"/>
-      <c r="P110" s="56"/>
+      <c r="K110" s="42"/>
+      <c r="L110" s="50"/>
+      <c r="M110" s="51"/>
+      <c r="N110" s="55"/>
+      <c r="O110" s="56"/>
+      <c r="P110" s="57"/>
     </row>
     <row r="111" ht="34" customHeight="1" spans="1:16">
       <c r="A111" s="36"/>
@@ -12874,12 +12890,12 @@
       <c r="H111" s="29"/>
       <c r="I111" s="29"/>
       <c r="J111" s="37"/>
-      <c r="K111" s="41"/>
-      <c r="L111" s="49"/>
-      <c r="M111" s="50"/>
-      <c r="N111" s="54"/>
-      <c r="O111" s="55"/>
-      <c r="P111" s="56"/>
+      <c r="K111" s="42"/>
+      <c r="L111" s="50"/>
+      <c r="M111" s="51"/>
+      <c r="N111" s="55"/>
+      <c r="O111" s="56"/>
+      <c r="P111" s="57"/>
     </row>
     <row r="112" ht="34" customHeight="1" spans="1:16">
       <c r="A112" s="36"/>
@@ -12892,12 +12908,12 @@
       <c r="H112" s="29"/>
       <c r="I112" s="29"/>
       <c r="J112" s="37"/>
-      <c r="K112" s="41"/>
-      <c r="L112" s="49"/>
-      <c r="M112" s="50"/>
-      <c r="N112" s="54"/>
-      <c r="O112" s="55"/>
-      <c r="P112" s="56"/>
+      <c r="K112" s="42"/>
+      <c r="L112" s="50"/>
+      <c r="M112" s="51"/>
+      <c r="N112" s="55"/>
+      <c r="O112" s="56"/>
+      <c r="P112" s="57"/>
     </row>
     <row r="113" ht="34" customHeight="1" spans="1:16">
       <c r="A113" s="36"/>
@@ -12910,12 +12926,12 @@
       <c r="H113" s="29"/>
       <c r="I113" s="29"/>
       <c r="J113" s="37"/>
-      <c r="K113" s="41"/>
-      <c r="L113" s="49"/>
-      <c r="M113" s="50"/>
-      <c r="N113" s="54"/>
-      <c r="O113" s="55"/>
-      <c r="P113" s="56"/>
+      <c r="K113" s="42"/>
+      <c r="L113" s="50"/>
+      <c r="M113" s="51"/>
+      <c r="N113" s="55"/>
+      <c r="O113" s="56"/>
+      <c r="P113" s="57"/>
     </row>
     <row r="114" ht="34" customHeight="1" spans="1:16">
       <c r="A114" s="36"/>
@@ -12928,12 +12944,12 @@
       <c r="H114" s="29"/>
       <c r="I114" s="29"/>
       <c r="J114" s="37"/>
-      <c r="K114" s="41"/>
-      <c r="L114" s="49"/>
-      <c r="M114" s="50"/>
-      <c r="N114" s="54"/>
-      <c r="O114" s="55"/>
-      <c r="P114" s="56"/>
+      <c r="K114" s="42"/>
+      <c r="L114" s="50"/>
+      <c r="M114" s="51"/>
+      <c r="N114" s="55"/>
+      <c r="O114" s="56"/>
+      <c r="P114" s="57"/>
     </row>
     <row r="115" ht="34" customHeight="1" spans="1:16">
       <c r="A115" s="36"/>
@@ -12946,12 +12962,12 @@
       <c r="H115" s="29"/>
       <c r="I115" s="29"/>
       <c r="J115" s="37"/>
-      <c r="K115" s="41"/>
-      <c r="L115" s="49"/>
-      <c r="M115" s="50"/>
-      <c r="N115" s="54"/>
-      <c r="O115" s="55"/>
-      <c r="P115" s="56"/>
+      <c r="K115" s="42"/>
+      <c r="L115" s="50"/>
+      <c r="M115" s="51"/>
+      <c r="N115" s="55"/>
+      <c r="O115" s="56"/>
+      <c r="P115" s="57"/>
     </row>
     <row r="116" ht="34" customHeight="1" spans="1:16">
       <c r="A116" s="22"/>
@@ -12964,12 +12980,12 @@
       <c r="H116" s="29"/>
       <c r="I116" s="29"/>
       <c r="J116" s="37"/>
-      <c r="K116" s="41"/>
-      <c r="L116" s="49"/>
-      <c r="M116" s="50"/>
-      <c r="N116" s="54"/>
-      <c r="O116" s="55"/>
-      <c r="P116" s="56"/>
+      <c r="K116" s="42"/>
+      <c r="L116" s="50"/>
+      <c r="M116" s="51"/>
+      <c r="N116" s="55"/>
+      <c r="O116" s="56"/>
+      <c r="P116" s="57"/>
     </row>
     <row r="117" ht="34" customHeight="1" spans="1:16">
       <c r="A117" s="22"/>
@@ -12982,12 +12998,12 @@
       <c r="H117" s="29"/>
       <c r="I117" s="29"/>
       <c r="J117" s="37"/>
-      <c r="K117" s="41"/>
-      <c r="L117" s="49"/>
-      <c r="M117" s="50"/>
-      <c r="N117" s="54"/>
-      <c r="O117" s="55"/>
-      <c r="P117" s="56"/>
+      <c r="K117" s="42"/>
+      <c r="L117" s="50"/>
+      <c r="M117" s="51"/>
+      <c r="N117" s="55"/>
+      <c r="O117" s="56"/>
+      <c r="P117" s="57"/>
     </row>
     <row r="118" ht="34" customHeight="1" spans="1:16">
       <c r="A118" s="22"/>
@@ -13000,12 +13016,12 @@
       <c r="H118" s="29"/>
       <c r="I118" s="29"/>
       <c r="J118" s="37"/>
-      <c r="K118" s="41"/>
-      <c r="L118" s="49"/>
-      <c r="M118" s="50"/>
-      <c r="N118" s="54"/>
-      <c r="O118" s="55"/>
-      <c r="P118" s="56"/>
+      <c r="K118" s="42"/>
+      <c r="L118" s="50"/>
+      <c r="M118" s="51"/>
+      <c r="N118" s="55"/>
+      <c r="O118" s="56"/>
+      <c r="P118" s="57"/>
     </row>
     <row r="119" ht="34" customHeight="1" spans="1:16">
       <c r="A119" s="22"/>
@@ -13018,12 +13034,12 @@
       <c r="H119" s="29"/>
       <c r="I119" s="29"/>
       <c r="J119" s="37"/>
-      <c r="K119" s="41"/>
-      <c r="L119" s="49"/>
-      <c r="M119" s="50"/>
-      <c r="N119" s="54"/>
-      <c r="O119" s="55"/>
-      <c r="P119" s="56"/>
+      <c r="K119" s="42"/>
+      <c r="L119" s="50"/>
+      <c r="M119" s="51"/>
+      <c r="N119" s="55"/>
+      <c r="O119" s="56"/>
+      <c r="P119" s="57"/>
     </row>
     <row r="120" ht="34" customHeight="1" spans="1:16">
       <c r="A120" s="36"/>
@@ -13036,12 +13052,12 @@
       <c r="H120" s="29"/>
       <c r="I120" s="29"/>
       <c r="J120" s="37"/>
-      <c r="K120" s="41"/>
-      <c r="L120" s="49"/>
-      <c r="M120" s="50"/>
-      <c r="N120" s="54"/>
-      <c r="O120" s="55"/>
-      <c r="P120" s="56"/>
+      <c r="K120" s="42"/>
+      <c r="L120" s="50"/>
+      <c r="M120" s="51"/>
+      <c r="N120" s="55"/>
+      <c r="O120" s="56"/>
+      <c r="P120" s="57"/>
     </row>
     <row r="121" ht="34" customHeight="1" spans="1:16">
       <c r="A121" s="36"/>
@@ -13054,12 +13070,12 @@
       <c r="H121" s="29"/>
       <c r="I121" s="29"/>
       <c r="J121" s="37"/>
-      <c r="K121" s="41"/>
-      <c r="L121" s="49"/>
-      <c r="M121" s="50"/>
-      <c r="N121" s="54"/>
-      <c r="O121" s="55"/>
-      <c r="P121" s="56"/>
+      <c r="K121" s="42"/>
+      <c r="L121" s="50"/>
+      <c r="M121" s="51"/>
+      <c r="N121" s="55"/>
+      <c r="O121" s="56"/>
+      <c r="P121" s="57"/>
     </row>
     <row r="122" ht="34" customHeight="1" spans="1:16">
       <c r="A122" s="22"/>
@@ -13072,12 +13088,12 @@
       <c r="H122" s="29"/>
       <c r="I122" s="29"/>
       <c r="J122" s="37"/>
-      <c r="K122" s="41"/>
-      <c r="L122" s="49"/>
-      <c r="M122" s="50"/>
-      <c r="N122" s="54"/>
-      <c r="O122" s="55"/>
-      <c r="P122" s="56"/>
+      <c r="K122" s="42"/>
+      <c r="L122" s="50"/>
+      <c r="M122" s="51"/>
+      <c r="N122" s="55"/>
+      <c r="O122" s="56"/>
+      <c r="P122" s="57"/>
     </row>
     <row r="123" ht="34" customHeight="1" spans="1:16">
       <c r="A123" s="22"/>
@@ -13090,12 +13106,12 @@
       <c r="H123" s="29"/>
       <c r="I123" s="29"/>
       <c r="J123" s="37"/>
-      <c r="K123" s="41"/>
-      <c r="L123" s="49"/>
-      <c r="M123" s="50"/>
-      <c r="N123" s="54"/>
-      <c r="O123" s="55"/>
-      <c r="P123" s="56"/>
+      <c r="K123" s="42"/>
+      <c r="L123" s="50"/>
+      <c r="M123" s="51"/>
+      <c r="N123" s="55"/>
+      <c r="O123" s="56"/>
+      <c r="P123" s="57"/>
     </row>
     <row r="124" ht="34" customHeight="1" spans="1:16">
       <c r="A124" s="22"/>
@@ -13108,12 +13124,12 @@
       <c r="H124" s="29"/>
       <c r="I124" s="29"/>
       <c r="J124" s="37"/>
-      <c r="K124" s="41"/>
-      <c r="L124" s="49"/>
-      <c r="M124" s="50"/>
-      <c r="N124" s="54"/>
-      <c r="O124" s="55"/>
-      <c r="P124" s="56"/>
+      <c r="K124" s="42"/>
+      <c r="L124" s="50"/>
+      <c r="M124" s="51"/>
+      <c r="N124" s="55"/>
+      <c r="O124" s="56"/>
+      <c r="P124" s="57"/>
     </row>
     <row r="125" ht="34" customHeight="1" spans="1:16">
       <c r="A125" s="36"/>
@@ -13126,12 +13142,12 @@
       <c r="H125" s="29"/>
       <c r="I125" s="29"/>
       <c r="J125" s="37"/>
-      <c r="K125" s="41"/>
-      <c r="L125" s="49"/>
-      <c r="M125" s="50"/>
-      <c r="N125" s="54"/>
-      <c r="O125" s="55"/>
-      <c r="P125" s="56"/>
+      <c r="K125" s="42"/>
+      <c r="L125" s="50"/>
+      <c r="M125" s="51"/>
+      <c r="N125" s="55"/>
+      <c r="O125" s="56"/>
+      <c r="P125" s="57"/>
     </row>
     <row r="126" ht="34" customHeight="1" spans="1:16">
       <c r="A126" s="36"/>
@@ -13144,12 +13160,12 @@
       <c r="H126" s="29"/>
       <c r="I126" s="29"/>
       <c r="J126" s="37"/>
-      <c r="K126" s="41"/>
-      <c r="L126" s="49"/>
-      <c r="M126" s="50"/>
-      <c r="N126" s="54"/>
-      <c r="O126" s="55"/>
-      <c r="P126" s="56"/>
+      <c r="K126" s="42"/>
+      <c r="L126" s="50"/>
+      <c r="M126" s="51"/>
+      <c r="N126" s="55"/>
+      <c r="O126" s="56"/>
+      <c r="P126" s="57"/>
     </row>
     <row r="127" ht="34" customHeight="1" spans="1:16">
       <c r="A127" s="36"/>
@@ -13162,12 +13178,12 @@
       <c r="H127" s="29"/>
       <c r="I127" s="29"/>
       <c r="J127" s="37"/>
-      <c r="K127" s="41"/>
-      <c r="L127" s="49"/>
-      <c r="M127" s="50"/>
-      <c r="N127" s="54"/>
-      <c r="O127" s="55"/>
-      <c r="P127" s="56"/>
+      <c r="K127" s="42"/>
+      <c r="L127" s="50"/>
+      <c r="M127" s="51"/>
+      <c r="N127" s="55"/>
+      <c r="O127" s="56"/>
+      <c r="P127" s="57"/>
     </row>
     <row r="128" ht="34" customHeight="1" spans="1:16">
       <c r="A128" s="36"/>
@@ -13180,12 +13196,12 @@
       <c r="H128" s="29"/>
       <c r="I128" s="29"/>
       <c r="J128" s="37"/>
-      <c r="K128" s="41"/>
-      <c r="L128" s="49"/>
-      <c r="M128" s="50"/>
-      <c r="N128" s="54"/>
-      <c r="O128" s="55"/>
-      <c r="P128" s="56"/>
+      <c r="K128" s="42"/>
+      <c r="L128" s="50"/>
+      <c r="M128" s="51"/>
+      <c r="N128" s="55"/>
+      <c r="O128" s="56"/>
+      <c r="P128" s="57"/>
     </row>
     <row r="129" ht="34" customHeight="1" spans="1:16">
       <c r="A129" s="36"/>
@@ -13198,12 +13214,12 @@
       <c r="H129" s="29"/>
       <c r="I129" s="29"/>
       <c r="J129" s="37"/>
-      <c r="K129" s="41"/>
-      <c r="L129" s="49"/>
-      <c r="M129" s="50"/>
-      <c r="N129" s="54"/>
-      <c r="O129" s="55"/>
-      <c r="P129" s="56"/>
+      <c r="K129" s="42"/>
+      <c r="L129" s="50"/>
+      <c r="M129" s="51"/>
+      <c r="N129" s="55"/>
+      <c r="O129" s="56"/>
+      <c r="P129" s="57"/>
     </row>
     <row r="130" ht="34" customHeight="1" spans="1:16">
       <c r="A130" s="36"/>
@@ -13216,12 +13232,12 @@
       <c r="H130" s="29"/>
       <c r="I130" s="29"/>
       <c r="J130" s="37"/>
-      <c r="K130" s="41"/>
-      <c r="L130" s="49"/>
-      <c r="M130" s="50"/>
-      <c r="N130" s="54"/>
-      <c r="O130" s="55"/>
-      <c r="P130" s="56"/>
+      <c r="K130" s="42"/>
+      <c r="L130" s="50"/>
+      <c r="M130" s="51"/>
+      <c r="N130" s="55"/>
+      <c r="O130" s="56"/>
+      <c r="P130" s="57"/>
     </row>
     <row r="131" ht="34" customHeight="1" spans="1:16">
       <c r="A131" s="36"/>
@@ -13234,12 +13250,12 @@
       <c r="H131" s="29"/>
       <c r="I131" s="29"/>
       <c r="J131" s="37"/>
-      <c r="K131" s="41"/>
-      <c r="L131" s="49"/>
-      <c r="M131" s="50"/>
-      <c r="N131" s="54"/>
-      <c r="O131" s="55"/>
-      <c r="P131" s="56"/>
+      <c r="K131" s="42"/>
+      <c r="L131" s="50"/>
+      <c r="M131" s="51"/>
+      <c r="N131" s="55"/>
+      <c r="O131" s="56"/>
+      <c r="P131" s="57"/>
     </row>
     <row r="132" ht="34" customHeight="1" spans="1:16">
       <c r="A132" s="36"/>
@@ -13252,12 +13268,12 @@
       <c r="H132" s="29"/>
       <c r="I132" s="29"/>
       <c r="J132" s="37"/>
-      <c r="K132" s="41"/>
-      <c r="L132" s="49"/>
-      <c r="M132" s="50"/>
-      <c r="N132" s="54"/>
-      <c r="O132" s="55"/>
-      <c r="P132" s="56"/>
+      <c r="K132" s="42"/>
+      <c r="L132" s="50"/>
+      <c r="M132" s="51"/>
+      <c r="N132" s="55"/>
+      <c r="O132" s="56"/>
+      <c r="P132" s="57"/>
     </row>
     <row r="133" ht="34" customHeight="1" spans="1:16">
       <c r="A133" s="36"/>
@@ -13270,12 +13286,12 @@
       <c r="H133" s="29"/>
       <c r="I133" s="29"/>
       <c r="J133" s="37"/>
-      <c r="K133" s="41"/>
-      <c r="L133" s="49"/>
-      <c r="M133" s="50"/>
-      <c r="N133" s="54"/>
-      <c r="O133" s="55"/>
-      <c r="P133" s="56"/>
+      <c r="K133" s="42"/>
+      <c r="L133" s="50"/>
+      <c r="M133" s="51"/>
+      <c r="N133" s="55"/>
+      <c r="O133" s="56"/>
+      <c r="P133" s="57"/>
     </row>
     <row r="134" ht="34" customHeight="1" spans="1:16">
       <c r="A134" s="36"/>
@@ -13288,12 +13304,12 @@
       <c r="H134" s="29"/>
       <c r="I134" s="29"/>
       <c r="J134" s="37"/>
-      <c r="K134" s="41"/>
-      <c r="L134" s="49"/>
-      <c r="M134" s="50"/>
-      <c r="N134" s="54"/>
-      <c r="O134" s="55"/>
-      <c r="P134" s="56"/>
+      <c r="K134" s="42"/>
+      <c r="L134" s="50"/>
+      <c r="M134" s="51"/>
+      <c r="N134" s="55"/>
+      <c r="O134" s="56"/>
+      <c r="P134" s="57"/>
     </row>
     <row r="135" ht="34" customHeight="1" spans="1:16">
       <c r="A135" s="36"/>
@@ -13306,12 +13322,12 @@
       <c r="H135" s="29"/>
       <c r="I135" s="29"/>
       <c r="J135" s="37"/>
-      <c r="K135" s="41"/>
-      <c r="L135" s="49"/>
-      <c r="M135" s="50"/>
-      <c r="N135" s="54"/>
-      <c r="O135" s="55"/>
-      <c r="P135" s="56"/>
+      <c r="K135" s="42"/>
+      <c r="L135" s="50"/>
+      <c r="M135" s="51"/>
+      <c r="N135" s="55"/>
+      <c r="O135" s="56"/>
+      <c r="P135" s="57"/>
     </row>
     <row r="136" ht="34" customHeight="1" spans="1:16">
       <c r="A136" s="36"/>
@@ -13324,12 +13340,12 @@
       <c r="H136" s="29"/>
       <c r="I136" s="29"/>
       <c r="J136" s="37"/>
-      <c r="K136" s="41"/>
-      <c r="L136" s="49"/>
-      <c r="M136" s="50"/>
-      <c r="N136" s="54"/>
-      <c r="O136" s="55"/>
-      <c r="P136" s="56"/>
+      <c r="K136" s="42"/>
+      <c r="L136" s="50"/>
+      <c r="M136" s="51"/>
+      <c r="N136" s="55"/>
+      <c r="O136" s="56"/>
+      <c r="P136" s="57"/>
     </row>
     <row r="137" ht="34" customHeight="1" spans="1:16">
       <c r="A137" s="36"/>
@@ -13342,12 +13358,12 @@
       <c r="H137" s="29"/>
       <c r="I137" s="29"/>
       <c r="J137" s="37"/>
-      <c r="K137" s="41"/>
-      <c r="L137" s="49"/>
-      <c r="M137" s="50"/>
-      <c r="N137" s="54"/>
-      <c r="O137" s="55"/>
-      <c r="P137" s="56"/>
+      <c r="K137" s="42"/>
+      <c r="L137" s="50"/>
+      <c r="M137" s="51"/>
+      <c r="N137" s="55"/>
+      <c r="O137" s="56"/>
+      <c r="P137" s="57"/>
     </row>
     <row r="138" ht="34" customHeight="1" spans="1:16">
       <c r="A138" s="36"/>
@@ -13360,12 +13376,12 @@
       <c r="H138" s="29"/>
       <c r="I138" s="29"/>
       <c r="J138" s="37"/>
-      <c r="K138" s="41"/>
-      <c r="L138" s="49"/>
-      <c r="M138" s="50"/>
-      <c r="N138" s="54"/>
-      <c r="O138" s="55"/>
-      <c r="P138" s="56"/>
+      <c r="K138" s="42"/>
+      <c r="L138" s="50"/>
+      <c r="M138" s="51"/>
+      <c r="N138" s="55"/>
+      <c r="O138" s="56"/>
+      <c r="P138" s="57"/>
     </row>
     <row r="139" s="1" customFormat="1" ht="23" customHeight="1" spans="1:16">
       <c r="A139" s="36"/>
@@ -15889,7 +15905,7 @@
     </row>
     <row r="281" ht="23" customHeight="1" spans="1:15">
       <c r="A281" s="36"/>
-      <c r="B281" s="39"/>
+      <c r="B281" s="40"/>
       <c r="C281" s="28"/>
       <c r="D281" s="29"/>
       <c r="E281" s="29"/>
@@ -15898,15 +15914,15 @@
       <c r="H281" s="29"/>
       <c r="I281" s="29"/>
       <c r="J281" s="37"/>
-      <c r="K281" s="41"/>
-      <c r="L281" s="49"/>
-      <c r="M281" s="50"/>
-      <c r="N281" s="49"/>
-      <c r="O281" s="41"/>
+      <c r="K281" s="42"/>
+      <c r="L281" s="50"/>
+      <c r="M281" s="51"/>
+      <c r="N281" s="50"/>
+      <c r="O281" s="42"/>
     </row>
     <row r="282" ht="23" customHeight="1" spans="1:15">
       <c r="A282" s="36"/>
-      <c r="B282" s="39"/>
+      <c r="B282" s="40"/>
       <c r="C282" s="28"/>
       <c r="D282" s="29"/>
       <c r="E282" s="29"/>
@@ -15915,15 +15931,15 @@
       <c r="H282" s="29"/>
       <c r="I282" s="29"/>
       <c r="J282" s="37"/>
-      <c r="K282" s="41"/>
-      <c r="L282" s="49"/>
-      <c r="M282" s="50"/>
-      <c r="N282" s="49"/>
-      <c r="O282" s="41"/>
+      <c r="K282" s="42"/>
+      <c r="L282" s="50"/>
+      <c r="M282" s="51"/>
+      <c r="N282" s="50"/>
+      <c r="O282" s="42"/>
     </row>
     <row r="283" ht="23" customHeight="1" spans="1:15">
       <c r="A283" s="36"/>
-      <c r="B283" s="39"/>
+      <c r="B283" s="40"/>
       <c r="C283" s="28"/>
       <c r="D283" s="29"/>
       <c r="E283" s="29"/>
@@ -15932,15 +15948,15 @@
       <c r="H283" s="29"/>
       <c r="I283" s="29"/>
       <c r="J283" s="37"/>
-      <c r="K283" s="41"/>
-      <c r="L283" s="49"/>
-      <c r="M283" s="50"/>
-      <c r="N283" s="49"/>
-      <c r="O283" s="41"/>
+      <c r="K283" s="42"/>
+      <c r="L283" s="50"/>
+      <c r="M283" s="51"/>
+      <c r="N283" s="50"/>
+      <c r="O283" s="42"/>
     </row>
     <row r="284" ht="23" customHeight="1" spans="1:15">
       <c r="A284" s="36"/>
-      <c r="B284" s="39"/>
+      <c r="B284" s="40"/>
       <c r="C284" s="28"/>
       <c r="D284" s="29"/>
       <c r="E284" s="29"/>
@@ -15949,15 +15965,15 @@
       <c r="H284" s="29"/>
       <c r="I284" s="29"/>
       <c r="J284" s="37"/>
-      <c r="K284" s="41"/>
-      <c r="L284" s="49"/>
-      <c r="M284" s="50"/>
-      <c r="N284" s="49"/>
-      <c r="O284" s="41"/>
+      <c r="K284" s="42"/>
+      <c r="L284" s="50"/>
+      <c r="M284" s="51"/>
+      <c r="N284" s="50"/>
+      <c r="O284" s="42"/>
     </row>
     <row r="285" ht="23" customHeight="1" spans="1:15">
       <c r="A285" s="36"/>
-      <c r="B285" s="39"/>
+      <c r="B285" s="40"/>
       <c r="C285" s="28"/>
       <c r="D285" s="29"/>
       <c r="E285" s="29"/>
@@ -15966,15 +15982,15 @@
       <c r="H285" s="29"/>
       <c r="I285" s="29"/>
       <c r="J285" s="37"/>
-      <c r="K285" s="41"/>
-      <c r="L285" s="49"/>
-      <c r="M285" s="50"/>
-      <c r="N285" s="49"/>
-      <c r="O285" s="41"/>
+      <c r="K285" s="42"/>
+      <c r="L285" s="50"/>
+      <c r="M285" s="51"/>
+      <c r="N285" s="50"/>
+      <c r="O285" s="42"/>
     </row>
     <row r="286" ht="23" customHeight="1" spans="1:15">
       <c r="A286" s="36"/>
-      <c r="B286" s="39"/>
+      <c r="B286" s="40"/>
       <c r="C286" s="28"/>
       <c r="D286" s="29"/>
       <c r="E286" s="29"/>
@@ -15983,15 +15999,15 @@
       <c r="H286" s="29"/>
       <c r="I286" s="29"/>
       <c r="J286" s="37"/>
-      <c r="K286" s="41"/>
-      <c r="L286" s="49"/>
-      <c r="M286" s="50"/>
-      <c r="N286" s="49"/>
-      <c r="O286" s="41"/>
+      <c r="K286" s="42"/>
+      <c r="L286" s="50"/>
+      <c r="M286" s="51"/>
+      <c r="N286" s="50"/>
+      <c r="O286" s="42"/>
     </row>
     <row r="287" ht="23" customHeight="1" spans="1:15">
       <c r="A287" s="36"/>
-      <c r="B287" s="39"/>
+      <c r="B287" s="40"/>
       <c r="C287" s="28"/>
       <c r="D287" s="29"/>
       <c r="E287" s="29"/>
@@ -16000,15 +16016,15 @@
       <c r="H287" s="29"/>
       <c r="I287" s="29"/>
       <c r="J287" s="37"/>
-      <c r="K287" s="41"/>
-      <c r="L287" s="49"/>
-      <c r="M287" s="50"/>
-      <c r="N287" s="49"/>
-      <c r="O287" s="41"/>
+      <c r="K287" s="42"/>
+      <c r="L287" s="50"/>
+      <c r="M287" s="51"/>
+      <c r="N287" s="50"/>
+      <c r="O287" s="42"/>
     </row>
     <row r="288" ht="23" customHeight="1" spans="1:15">
       <c r="A288" s="36"/>
-      <c r="B288" s="39"/>
+      <c r="B288" s="40"/>
       <c r="C288" s="28"/>
       <c r="D288" s="29"/>
       <c r="E288" s="29"/>
@@ -16017,15 +16033,15 @@
       <c r="H288" s="29"/>
       <c r="I288" s="29"/>
       <c r="J288" s="37"/>
-      <c r="K288" s="41"/>
-      <c r="L288" s="49"/>
-      <c r="M288" s="50"/>
-      <c r="N288" s="49"/>
-      <c r="O288" s="41"/>
+      <c r="K288" s="42"/>
+      <c r="L288" s="50"/>
+      <c r="M288" s="51"/>
+      <c r="N288" s="50"/>
+      <c r="O288" s="42"/>
     </row>
     <row r="289" ht="23" customHeight="1" spans="1:15">
       <c r="A289" s="36"/>
-      <c r="B289" s="39"/>
+      <c r="B289" s="40"/>
       <c r="C289" s="28"/>
       <c r="D289" s="29"/>
       <c r="E289" s="29"/>
@@ -16034,15 +16050,15 @@
       <c r="H289" s="29"/>
       <c r="I289" s="29"/>
       <c r="J289" s="37"/>
-      <c r="K289" s="41"/>
-      <c r="L289" s="49"/>
-      <c r="M289" s="50"/>
-      <c r="N289" s="49"/>
-      <c r="O289" s="41"/>
+      <c r="K289" s="42"/>
+      <c r="L289" s="50"/>
+      <c r="M289" s="51"/>
+      <c r="N289" s="50"/>
+      <c r="O289" s="42"/>
     </row>
     <row r="290" ht="23" customHeight="1" spans="1:15">
       <c r="A290" s="36"/>
-      <c r="B290" s="39"/>
+      <c r="B290" s="40"/>
       <c r="C290" s="28"/>
       <c r="D290" s="29"/>
       <c r="E290" s="29"/>
@@ -16051,15 +16067,15 @@
       <c r="H290" s="29"/>
       <c r="I290" s="29"/>
       <c r="J290" s="37"/>
-      <c r="K290" s="41"/>
-      <c r="L290" s="49"/>
-      <c r="M290" s="50"/>
-      <c r="N290" s="49"/>
-      <c r="O290" s="41"/>
+      <c r="K290" s="42"/>
+      <c r="L290" s="50"/>
+      <c r="M290" s="51"/>
+      <c r="N290" s="50"/>
+      <c r="O290" s="42"/>
     </row>
     <row r="291" ht="23" customHeight="1" spans="1:15">
       <c r="A291" s="36"/>
-      <c r="B291" s="39"/>
+      <c r="B291" s="40"/>
       <c r="C291" s="28"/>
       <c r="D291" s="29"/>
       <c r="E291" s="29"/>
@@ -16068,15 +16084,15 @@
       <c r="H291" s="29"/>
       <c r="I291" s="29"/>
       <c r="J291" s="37"/>
-      <c r="K291" s="41"/>
-      <c r="L291" s="49"/>
-      <c r="M291" s="50"/>
-      <c r="N291" s="49"/>
-      <c r="O291" s="41"/>
+      <c r="K291" s="42"/>
+      <c r="L291" s="50"/>
+      <c r="M291" s="51"/>
+      <c r="N291" s="50"/>
+      <c r="O291" s="42"/>
     </row>
     <row r="292" ht="23" customHeight="1" spans="1:15">
       <c r="A292" s="36"/>
-      <c r="B292" s="39"/>
+      <c r="B292" s="40"/>
       <c r="C292" s="28"/>
       <c r="D292" s="29"/>
       <c r="E292" s="29"/>
@@ -16085,15 +16101,15 @@
       <c r="H292" s="29"/>
       <c r="I292" s="29"/>
       <c r="J292" s="37"/>
-      <c r="K292" s="41"/>
-      <c r="L292" s="49"/>
-      <c r="M292" s="50"/>
-      <c r="N292" s="49"/>
-      <c r="O292" s="41"/>
+      <c r="K292" s="42"/>
+      <c r="L292" s="50"/>
+      <c r="M292" s="51"/>
+      <c r="N292" s="50"/>
+      <c r="O292" s="42"/>
     </row>
     <row r="293" ht="23" customHeight="1" spans="1:15">
       <c r="A293" s="36"/>
-      <c r="B293" s="39"/>
+      <c r="B293" s="40"/>
       <c r="C293" s="28"/>
       <c r="D293" s="29"/>
       <c r="E293" s="29"/>
@@ -16102,15 +16118,15 @@
       <c r="H293" s="29"/>
       <c r="I293" s="29"/>
       <c r="J293" s="37"/>
-      <c r="K293" s="41"/>
-      <c r="L293" s="49"/>
-      <c r="M293" s="50"/>
-      <c r="N293" s="49"/>
-      <c r="O293" s="41"/>
+      <c r="K293" s="42"/>
+      <c r="L293" s="50"/>
+      <c r="M293" s="51"/>
+      <c r="N293" s="50"/>
+      <c r="O293" s="42"/>
     </row>
     <row r="294" ht="23" customHeight="1" spans="1:15">
       <c r="A294" s="36"/>
-      <c r="B294" s="39"/>
+      <c r="B294" s="40"/>
       <c r="C294" s="28"/>
       <c r="D294" s="29"/>
       <c r="E294" s="29"/>
@@ -16119,15 +16135,15 @@
       <c r="H294" s="29"/>
       <c r="I294" s="29"/>
       <c r="J294" s="37"/>
-      <c r="K294" s="41"/>
-      <c r="L294" s="49"/>
-      <c r="M294" s="50"/>
-      <c r="N294" s="49"/>
-      <c r="O294" s="41"/>
+      <c r="K294" s="42"/>
+      <c r="L294" s="50"/>
+      <c r="M294" s="51"/>
+      <c r="N294" s="50"/>
+      <c r="O294" s="42"/>
     </row>
     <row r="295" ht="23" customHeight="1" spans="1:15">
       <c r="A295" s="36"/>
-      <c r="B295" s="39"/>
+      <c r="B295" s="40"/>
       <c r="C295" s="28"/>
       <c r="D295" s="29"/>
       <c r="E295" s="29"/>
@@ -16136,15 +16152,15 @@
       <c r="H295" s="29"/>
       <c r="I295" s="29"/>
       <c r="J295" s="37"/>
-      <c r="K295" s="41"/>
-      <c r="L295" s="49"/>
-      <c r="M295" s="50"/>
-      <c r="N295" s="49"/>
-      <c r="O295" s="41"/>
+      <c r="K295" s="42"/>
+      <c r="L295" s="50"/>
+      <c r="M295" s="51"/>
+      <c r="N295" s="50"/>
+      <c r="O295" s="42"/>
     </row>
     <row r="296" ht="23" customHeight="1" spans="1:15">
       <c r="A296" s="36"/>
-      <c r="B296" s="39"/>
+      <c r="B296" s="40"/>
       <c r="C296" s="28"/>
       <c r="D296" s="29"/>
       <c r="E296" s="29"/>
@@ -16153,15 +16169,15 @@
       <c r="H296" s="29"/>
       <c r="I296" s="29"/>
       <c r="J296" s="37"/>
-      <c r="K296" s="41"/>
-      <c r="L296" s="49"/>
-      <c r="M296" s="50"/>
-      <c r="N296" s="49"/>
-      <c r="O296" s="41"/>
+      <c r="K296" s="42"/>
+      <c r="L296" s="50"/>
+      <c r="M296" s="51"/>
+      <c r="N296" s="50"/>
+      <c r="O296" s="42"/>
     </row>
     <row r="297" ht="23" customHeight="1" spans="1:15">
       <c r="A297" s="36"/>
-      <c r="B297" s="39"/>
+      <c r="B297" s="40"/>
       <c r="C297" s="28"/>
       <c r="D297" s="29"/>
       <c r="E297" s="29"/>
@@ -16170,15 +16186,15 @@
       <c r="H297" s="29"/>
       <c r="I297" s="29"/>
       <c r="J297" s="37"/>
-      <c r="K297" s="41"/>
-      <c r="L297" s="49"/>
-      <c r="M297" s="50"/>
-      <c r="N297" s="49"/>
-      <c r="O297" s="41"/>
+      <c r="K297" s="42"/>
+      <c r="L297" s="50"/>
+      <c r="M297" s="51"/>
+      <c r="N297" s="50"/>
+      <c r="O297" s="42"/>
     </row>
     <row r="298" ht="23" customHeight="1" spans="1:15">
       <c r="A298" s="36"/>
-      <c r="B298" s="39"/>
+      <c r="B298" s="40"/>
       <c r="C298" s="28"/>
       <c r="D298" s="29"/>
       <c r="E298" s="29"/>
@@ -16187,15 +16203,15 @@
       <c r="H298" s="29"/>
       <c r="I298" s="29"/>
       <c r="J298" s="37"/>
-      <c r="K298" s="41"/>
-      <c r="L298" s="49"/>
-      <c r="M298" s="50"/>
-      <c r="N298" s="49"/>
-      <c r="O298" s="41"/>
+      <c r="K298" s="42"/>
+      <c r="L298" s="50"/>
+      <c r="M298" s="51"/>
+      <c r="N298" s="50"/>
+      <c r="O298" s="42"/>
     </row>
     <row r="299" ht="23" customHeight="1" spans="1:15">
       <c r="A299" s="36"/>
-      <c r="B299" s="39"/>
+      <c r="B299" s="40"/>
       <c r="C299" s="28"/>
       <c r="D299" s="29"/>
       <c r="E299" s="29"/>
@@ -16204,11 +16220,11 @@
       <c r="H299" s="29"/>
       <c r="I299" s="29"/>
       <c r="J299" s="37"/>
-      <c r="K299" s="41"/>
-      <c r="L299" s="49"/>
-      <c r="M299" s="50"/>
-      <c r="N299" s="49"/>
-      <c r="O299" s="41"/>
+      <c r="K299" s="42"/>
+      <c r="L299" s="50"/>
+      <c r="M299" s="51"/>
+      <c r="N299" s="50"/>
+      <c r="O299" s="42"/>
     </row>
   </sheetData>
   <sheetProtection insertRows="0" insertHyperlinks="0" deleteRows="0"/>

</xml_diff>